<commit_message>
add form import from excel
</commit_message>
<xml_diff>
--- a/books.xlsx
+++ b/books.xlsx
@@ -1,25 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="24816"/>
-  <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
+  <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
+  <workbookPr/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16180" tabRatio="500"/>
+    <workbookView windowWidth="20400" windowHeight="8400" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="140000" concurrentCalc="0"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
-      <mx:ArchID Flags="2"/>
-    </ext>
-  </extLst>
+  <calcPr calcId="144525" concurrentCalc="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30">
   <si>
     <t>Book</t>
   </si>
@@ -27,12 +22,12 @@
     <t>id</t>
   </si>
   <si>
+    <t>title</t>
+  </si>
+  <si>
     <t>author</t>
   </si>
   <si>
-    <t>title</t>
-  </si>
-  <si>
     <t>description</t>
   </si>
   <si>
@@ -45,80 +40,94 @@
     <t>Buku 1</t>
   </si>
   <si>
+    <t>Penulis 1</t>
+  </si>
+  <si>
+    <t>Deskripsi 1</t>
+  </si>
+  <si>
+    <t>cover.png</t>
+  </si>
+  <si>
     <t>Buku 2</t>
   </si>
   <si>
+    <t>Penulis 2</t>
+  </si>
+  <si>
+    <t>Deskripsi 2</t>
+  </si>
+  <si>
     <t>Buku 3</t>
   </si>
   <si>
+    <t>Penulis 3</t>
+  </si>
+  <si>
+    <t>Deskripsi 3</t>
+  </si>
+  <si>
     <t>Buku 4</t>
   </si>
   <si>
+    <t>Penulis 4</t>
+  </si>
+  <si>
+    <t>Deskripsi 4</t>
+  </si>
+  <si>
     <t>Buku 5</t>
   </si>
   <si>
+    <t>Penulis 5</t>
+  </si>
+  <si>
+    <t>Deskripsi 5</t>
+  </si>
+  <si>
     <t>Buku 6</t>
   </si>
   <si>
+    <t>Penulis 6</t>
+  </si>
+  <si>
+    <t>Deskripsi 6</t>
+  </si>
+  <si>
     <t>Buku 7</t>
   </si>
   <si>
-    <t>Penulis 1</t>
-  </si>
-  <si>
-    <t>Penulis 2</t>
-  </si>
-  <si>
-    <t>Penulis 3</t>
-  </si>
-  <si>
-    <t>Penulis 4</t>
-  </si>
-  <si>
-    <t>Penulis 5</t>
-  </si>
-  <si>
-    <t>Penulis 6</t>
-  </si>
-  <si>
     <t>Penulis 7</t>
   </si>
   <si>
-    <t>Deskripsi 1</t>
-  </si>
-  <si>
-    <t>Deskripsi 2</t>
-  </si>
-  <si>
-    <t>Deskripsi 3</t>
-  </si>
-  <si>
-    <t>Deskripsi 4</t>
-  </si>
-  <si>
-    <t>Deskripsi 5</t>
-  </si>
-  <si>
-    <t>Deskripsi 6</t>
-  </si>
-  <si>
     <t>Deskripsi 7</t>
   </si>
   <si>
-    <t>cover.png</t>
+    <t>Buku 8</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="4">
+    <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
+    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+  </numFmts>
+  <fonts count="2">
     <font>
       <sz val="12"/>
-      <color theme="1"/>
+      <color indexed="63"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <scheme val="minor"/>
+      <charset val="134"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <name val="Arial"/>
+      <charset val="134"/>
     </font>
   </fonts>
   <fills count="2">
@@ -129,7 +138,14 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
     <border>
       <left/>
       <right/>
@@ -138,22 +154,42 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+  <cellStyleXfs count="6">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="1" fillId="0" borderId="1" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="1" fillId="0" borderId="1" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="1" fillId="0" borderId="1" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="1" fillId="0" borderId="1" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="1" fillId="0" borderId="1" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
   </cellStyleXfs>
   <cellXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="6">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Currency[0]" xfId="1" builtinId="7"/>
+    <cellStyle name="Percent" xfId="2" builtinId="5"/>
+    <cellStyle name="Comma" xfId="3" builtinId="3"/>
+    <cellStyle name="Currency" xfId="4" builtinId="4"/>
+    <cellStyle name="Comma[0]" xfId="5" builtinId="6"/>
   </cellStyles>
-  <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 主题​​">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -198,71 +234,71 @@
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Arab" typeface="Times New Roman"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Guru" typeface="Raavi"/>
         <a:font script="Hang" typeface="맑은 고딕"/>
         <a:font script="Hans" typeface="宋体"/>
         <a:font script="Hant" typeface="新細明體"/>
-        <a:font script="Arab" typeface="Times New Roman"/>
         <a:font script="Hebr" typeface="Times New Roman"/>
-        <a:font script="Thai" typeface="Tahoma"/>
-        <a:font script="Ethi" typeface="Nyala"/>
-        <a:font script="Beng" typeface="Vrinda"/>
-        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
         <a:font script="Khmr" typeface="MoolBoran"/>
         <a:font script="Knda" typeface="Tunga"/>
-        <a:font script="Guru" typeface="Raavi"/>
-        <a:font script="Cans" typeface="Euphemia"/>
-        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
-        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
-        <a:font script="Thaa" typeface="MV Boli"/>
-        <a:font script="Deva" typeface="Mangal"/>
-        <a:font script="Telu" typeface="Gautami"/>
-        <a:font script="Taml" typeface="Latha"/>
-        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
-        <a:font script="Orya" typeface="Kalinga"/>
-        <a:font script="Mlym" typeface="Kartika"/>
-        <a:font script="Laoo" typeface="DokChampa"/>
-        <a:font script="Sinh" typeface="Iskoola Pota"/>
-        <a:font script="Mong" typeface="Mongolian Baiti"/>
-        <a:font script="Viet" typeface="Times New Roman"/>
-        <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Arab" typeface="Arial"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Guru" typeface="Raavi"/>
         <a:font script="Hang" typeface="맑은 고딕"/>
         <a:font script="Hans" typeface="宋体"/>
         <a:font script="Hant" typeface="新細明體"/>
-        <a:font script="Arab" typeface="Arial"/>
         <a:font script="Hebr" typeface="Arial"/>
-        <a:font script="Thai" typeface="Tahoma"/>
-        <a:font script="Ethi" typeface="Nyala"/>
-        <a:font script="Beng" typeface="Vrinda"/>
-        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
         <a:font script="Khmr" typeface="DaunPenh"/>
         <a:font script="Knda" typeface="Tunga"/>
-        <a:font script="Guru" typeface="Raavi"/>
-        <a:font script="Cans" typeface="Euphemia"/>
-        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Viet" typeface="Arial"/>
         <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
-        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
-        <a:font script="Thaa" typeface="MV Boli"/>
-        <a:font script="Deva" typeface="Mangal"/>
-        <a:font script="Telu" typeface="Gautami"/>
-        <a:font script="Taml" typeface="Latha"/>
-        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
-        <a:font script="Orya" typeface="Kalinga"/>
-        <a:font script="Mlym" typeface="Kartika"/>
-        <a:font script="Laoo" typeface="DokChampa"/>
-        <a:font script="Sinh" typeface="Iskoola Pota"/>
-        <a:font script="Mong" typeface="Mongolian Baiti"/>
-        <a:font script="Viet" typeface="Arial"/>
-        <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -297,16 +333,20 @@
           <a:gsLst>
             <a:gs pos="0">
               <a:schemeClr val="phClr">
-                <a:tint val="100000"/>
-                <a:shade val="100000"/>
+                <a:shade val="51000"/>
                 <a:satMod val="130000"/>
               </a:schemeClr>
             </a:gs>
+            <a:gs pos="80000">
+              <a:schemeClr val="phClr">
+                <a:shade val="93000"/>
+                <a:satMod val="130000"/>
+              </a:schemeClr>
+            </a:gs>
             <a:gs pos="100000">
               <a:schemeClr val="phClr">
-                <a:tint val="50000"/>
-                <a:shade val="100000"/>
-                <a:satMod val="350000"/>
+                <a:shade val="94000"/>
+                <a:satMod val="135000"/>
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
@@ -391,8 +431,8 @@
             <a:gs pos="40000">
               <a:schemeClr val="phClr">
                 <a:tint val="45000"/>
+                <a:satMod val="350000"/>
                 <a:shade val="99000"/>
-                <a:satMod val="350000"/>
               </a:schemeClr>
             </a:gs>
             <a:gs pos="100000">
@@ -430,59 +470,71 @@
   </a:themeElements>
   <a:objectDefaults>
     <a:spDef>
-      <a:spPr/>
+      <a:spPr>
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="0" cy="0"/>
+        </a:xfrm>
+        <a:custGeom>
+          <a:avLst/>
+          <a:gdLst>
+            <a:gd name="_h" fmla="val 21600"/>
+            <a:gd name="_w" fmla="val 21600"/>
+          </a:gdLst>
+          <a:ahLst/>
+          <a:cxnLst/>
+          <a:pathLst>
+            <a:path w="21600" h="21600"/>
+          </a:pathLst>
+        </a:custGeom>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:srgbClr val="3E7FCD"/>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:srgbClr val="A3C2FF"/>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="16200000" scaled="0"/>
+        </a:gradFill>
+        <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:srgbClr val="4A7DBA">
+              <a:alpha val="100000"/>
+            </a:srgbClr>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:round/>
+        </a:ln>
+        <a:effectLst>
+          <a:outerShdw dist="23000" dir="5400000" rotWithShape="0">
+            <a:srgbClr val="000000">
+              <a:alpha val="35000"/>
+            </a:srgbClr>
+          </a:outerShdw>
+        </a:effectLst>
+      </a:spPr>
       <a:bodyPr/>
       <a:lstStyle/>
-      <a:style>
-        <a:lnRef idx="1">
-          <a:schemeClr val="accent1"/>
-        </a:lnRef>
-        <a:fillRef idx="3">
-          <a:schemeClr val="accent1"/>
-        </a:fillRef>
-        <a:effectRef idx="2">
-          <a:schemeClr val="accent1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="lt1"/>
-        </a:fontRef>
-      </a:style>
     </a:spDef>
-    <a:lnDef>
-      <a:spPr/>
-      <a:bodyPr/>
-      <a:lstStyle/>
-      <a:style>
-        <a:lnRef idx="2">
-          <a:schemeClr val="accent1"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:fillRef>
-        <a:effectRef idx="1">
-          <a:schemeClr val="accent1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="tx1"/>
-        </a:fontRef>
-      </a:style>
-    </a:lnDef>
   </a:objectDefaults>
   <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F9"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr/>
+  <dimension ref="A1:F10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I8" sqref="I8"/>
+      <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="17.05" outlineLevelCol="5"/>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:1">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -492,10 +544,10 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C2" t="s">
         <v>3</v>
-      </c>
-      <c r="C2" t="s">
-        <v>2</v>
       </c>
       <c r="D2" t="s">
         <v>4</v>
@@ -515,16 +567,16 @@
         <v>7</v>
       </c>
       <c r="C3" t="s">
-        <v>14</v>
+        <v>8</v>
       </c>
       <c r="D3" t="s">
-        <v>21</v>
+        <v>9</v>
       </c>
       <c r="E3">
         <v>1</v>
       </c>
       <c r="F3" t="s">
-        <v>28</v>
+        <v>10</v>
       </c>
     </row>
     <row r="4" spans="1:6">
@@ -532,19 +584,19 @@
         <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="C4" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="D4" t="s">
-        <v>22</v>
+        <v>13</v>
       </c>
       <c r="E4">
         <v>0</v>
       </c>
       <c r="F4" t="s">
-        <v>28</v>
+        <v>10</v>
       </c>
     </row>
     <row r="5" spans="1:6">
@@ -552,19 +604,19 @@
         <v>3</v>
       </c>
       <c r="B5" t="s">
-        <v>9</v>
+        <v>14</v>
       </c>
       <c r="C5" t="s">
+        <v>15</v>
+      </c>
+      <c r="D5" t="s">
         <v>16</v>
-      </c>
-      <c r="D5" t="s">
-        <v>23</v>
       </c>
       <c r="E5">
         <v>1</v>
       </c>
       <c r="F5" t="s">
-        <v>28</v>
+        <v>10</v>
       </c>
     </row>
     <row r="6" spans="1:6">
@@ -572,19 +624,19 @@
         <v>4</v>
       </c>
       <c r="B6" t="s">
-        <v>10</v>
+        <v>17</v>
       </c>
       <c r="C6" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="D6" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="E6">
         <v>0</v>
       </c>
       <c r="F6" t="s">
-        <v>28</v>
+        <v>10</v>
       </c>
     </row>
     <row r="7" spans="1:6">
@@ -592,19 +644,19 @@
         <v>5</v>
       </c>
       <c r="B7" t="s">
-        <v>11</v>
+        <v>20</v>
       </c>
       <c r="C7" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="D7" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="E7">
         <v>1</v>
       </c>
       <c r="F7" t="s">
-        <v>28</v>
+        <v>10</v>
       </c>
     </row>
     <row r="8" spans="1:6">
@@ -612,19 +664,19 @@
         <v>6</v>
       </c>
       <c r="B8" t="s">
-        <v>12</v>
+        <v>23</v>
       </c>
       <c r="C8" t="s">
-        <v>19</v>
+        <v>24</v>
       </c>
       <c r="D8" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="E8">
         <v>0</v>
       </c>
       <c r="F8" t="s">
-        <v>28</v>
+        <v>10</v>
       </c>
     </row>
     <row r="9" spans="1:6">
@@ -632,27 +684,44 @@
         <v>7</v>
       </c>
       <c r="B9" t="s">
-        <v>13</v>
+        <v>26</v>
       </c>
       <c r="C9" t="s">
-        <v>20</v>
+        <v>27</v>
       </c>
       <c r="D9" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="E9">
         <v>1</v>
       </c>
       <c r="F9" t="s">
-        <v>28</v>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6">
+      <c r="A10">
+        <v>8</v>
+      </c>
+      <c r="B10" t="s">
+        <v>29</v>
+      </c>
+      <c r="C10" t="s">
+        <v>8</v>
+      </c>
+      <c r="D10" t="s">
+        <v>9</v>
+      </c>
+      <c r="E10">
+        <v>0</v>
+      </c>
+      <c r="F10" t="s">
+        <v>10</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
+  <pageSetup paperSize="9" orientation="portrait"/>
+  <headerFooter alignWithMargins="0"/>
 </worksheet>
 </file>
</xml_diff>